<commit_message>
page object created for loginpage, mainpage
</commit_message>
<xml_diff>
--- a/target/Test Template Document Corp-TC-OH-17.xlsx
+++ b/target/Test Template Document Corp-TC-OH-17.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine\Company\CGI3\cucumber_workspace\OrangeAutomation\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1299,7 +1299,7 @@
         <xdr:cNvPr id="2154" name="Picture 2" descr="pcs">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2074,7 +2074,7 @@
   <dimension ref="A1:M387"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:G19"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75"/>
@@ -4005,6 +4005,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
+    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
+    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
+    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046351F880B96AE4B9BB4815879ADEBDD" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487f15db4e05f84fdb19aa3f548b93b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81372d4e-bcfc-4844-a57b-a09c5da71958" xmlns:ns3="952a6df7-b138-4f89-9bc4-e7a874ea3254" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09419ac551552483846d59652a820d17" ns2:_="" ns3:_="">
     <xsd:import namespace="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -4174,31 +4198,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
-    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
-    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
-    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E28044-843A-4D7D-9F1F-711CA3C23377}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4215,37 +4248,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
-    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>